<commit_message>
Update US African Revolt Timeline.xlsx
</commit_message>
<xml_diff>
--- a/US African Revolt Timeline.xlsx
+++ b/US African Revolt Timeline.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgroomes\Documents\Data Analytics\US African Revolt Timeline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgroomes\Documents\GitHub\USAfricanRevoltTimeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="44">
   <si>
     <t>Year</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>http://www.popflock.com/learn?s=Slave_revolt</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -488,7 +491,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,6 +772,9 @@
       <c r="C19" t="s">
         <v>10</v>
       </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
       <c r="E19" t="s">
         <v>15</v>
       </c>

</xml_diff>